<commit_message>
correct 2019 Santa Fe min wage
</commit_message>
<xml_diff>
--- a/rawdata/SubstateMinimumWage_Changes.xlsx
+++ b/rawdata/SubstateMinimumWage_Changes.xlsx
@@ -717,7 +717,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -770,18 +770,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -794,9 +790,9 @@
   <dimension ref="A1:S309"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A262" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="N305" activeCellId="0" sqref="N305"/>
+      <selection pane="bottomLeft" activeCell="D241" activeCellId="0" sqref="D241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7965,7 +7961,7 @@
       <c r="R201" s="8"/>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="13" t="n">
+      <c r="A202" s="1" t="n">
         <v>27</v>
       </c>
       <c r="B202" s="9" t="s">
@@ -8002,7 +7998,7 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="13" t="n">
+      <c r="A203" s="1" t="n">
         <v>27</v>
       </c>
       <c r="B203" s="9" t="s">
@@ -9376,7 +9372,7 @@
         <v>168</v>
       </c>
       <c r="D240" s="3" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="E240" s="3" t="n">
         <v>3</v>

</xml_diff>